<commit_message>
Update: BaseMachine Exio Board
</commit_message>
<xml_diff>
--- a/ベースマシン接続一覧表.xlsx
+++ b/ベースマシン接続一覧表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="176">
   <si>
     <t>ベースマシン接続一覧表</t>
     <rPh sb="6" eb="8">
@@ -524,148 +524,194 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Pattern8</t>
+  </si>
+  <si>
+    <t>Master</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>INTA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>INTB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SPI Bus Buffer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DCO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SPI IN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SPI OUT1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SPI OUT2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DCF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SPI OUT3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DCA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SW</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UIMode</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>EEPROM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SCL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SDA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RESET</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SW</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Slot_A</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Slot_B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Paste</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Copy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cancel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ok</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Load</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2017.01.06</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>Pattern2</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Pattern3</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Pattern4</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Pattern5</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Pattern6</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Pattern7</t>
-  </si>
-  <si>
-    <t>Pattern8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Save</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AT24C1024</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VCC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>WP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SCL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SDA</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Master</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>INTA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>INTB</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SPI Bus Buffer</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DCO</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SPI IN</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SPI OUT1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SPI OUT2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DCF</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SPI OUT3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DCA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SW</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>UIMode</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>EEPROM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>SCL</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SDA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>GND</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>RESET</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>RE</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SW</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Slot_A</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Slot_B</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Paste</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Copy</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Cancel</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Ok</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Load</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Save</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2016.12.21</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -699,7 +745,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -772,6 +818,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -802,7 +860,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -855,6 +913,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1154,10 +1227,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R111"/>
+  <dimension ref="A1:R118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1179,7 +1252,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1228,7 +1301,7 @@
       <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="9"/>
       <c r="E7" t="s">
         <v>24</v>
       </c>
@@ -1241,7 +1314,7 @@
       <c r="I7" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="12"/>
+      <c r="J7" s="8"/>
       <c r="K7" t="s">
         <v>24</v>
       </c>
@@ -1256,7 +1329,7 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="7"/>
       <c r="E8" t="s">
         <v>24</v>
       </c>
@@ -1269,7 +1342,7 @@
       <c r="I8" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="15"/>
+      <c r="J8" s="18"/>
       <c r="K8" t="s">
         <v>24</v>
       </c>
@@ -1314,7 +1387,7 @@
       <c r="I10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="8"/>
+      <c r="J10" s="15"/>
       <c r="K10" t="s">
         <v>24</v>
       </c>
@@ -1366,7 +1439,7 @@
       <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="12"/>
       <c r="E13" t="s">
         <v>24</v>
       </c>
@@ -1477,10 +1550,10 @@
       </c>
       <c r="D18" s="11"/>
       <c r="E18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F18" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H18">
         <v>24</v>
@@ -1721,12 +1794,12 @@
       <c r="C30" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="11"/>
+      <c r="D30" s="19"/>
       <c r="E30" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F30" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="H30">
         <v>4</v>
@@ -1749,12 +1822,12 @@
       <c r="C31" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="7"/>
+      <c r="D31" s="4"/>
       <c r="E31" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F31" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H31">
         <v>6</v>
@@ -1796,7 +1869,7 @@
         <v>57</v>
       </c>
       <c r="F33" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H33">
         <v>10</v>
@@ -2001,7 +2074,7 @@
         <v>57</v>
       </c>
       <c r="F41" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H41">
         <v>26</v>
@@ -2183,6 +2256,7 @@
       <c r="C51" t="s">
         <v>108</v>
       </c>
+      <c r="D51" s="11"/>
       <c r="E51" t="s">
         <v>26</v>
       </c>
@@ -2195,11 +2269,12 @@
       <c r="I51" t="s">
         <v>116</v>
       </c>
+      <c r="J51" s="5"/>
       <c r="K51" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="L51" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -2209,11 +2284,12 @@
       <c r="C52" t="s">
         <v>109</v>
       </c>
+      <c r="D52" s="10"/>
       <c r="E52" t="s">
         <v>26</v>
       </c>
       <c r="F52" t="s">
-        <v>128</v>
+        <v>161</v>
       </c>
       <c r="H52">
         <v>27</v>
@@ -2221,11 +2297,12 @@
       <c r="I52" t="s">
         <v>117</v>
       </c>
+      <c r="J52" s="4"/>
       <c r="K52" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="L52" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -2235,11 +2312,12 @@
       <c r="C53" t="s">
         <v>110</v>
       </c>
+      <c r="D53" s="7"/>
       <c r="E53" t="s">
         <v>26</v>
       </c>
       <c r="F53" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="H53">
         <v>26</v>
@@ -2247,11 +2325,12 @@
       <c r="I53" t="s">
         <v>118</v>
       </c>
+      <c r="J53" s="2"/>
       <c r="K53" t="s">
+        <v>149</v>
+      </c>
+      <c r="L53" t="s">
         <v>156</v>
-      </c>
-      <c r="L53" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -2261,11 +2340,12 @@
       <c r="C54" t="s">
         <v>111</v>
       </c>
+      <c r="D54" s="8"/>
       <c r="E54" t="s">
         <v>26</v>
       </c>
       <c r="F54" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="H54">
         <v>25</v>
@@ -2273,11 +2353,12 @@
       <c r="I54" t="s">
         <v>119</v>
       </c>
+      <c r="J54" s="12"/>
       <c r="K54" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="L54" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -2287,11 +2368,12 @@
       <c r="C55" t="s">
         <v>112</v>
       </c>
+      <c r="D55" s="12"/>
       <c r="E55" t="s">
         <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="H55">
         <v>24</v>
@@ -2299,11 +2381,12 @@
       <c r="I55" t="s">
         <v>120</v>
       </c>
+      <c r="J55" s="8"/>
       <c r="K55" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="L55" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -2313,11 +2396,12 @@
       <c r="C56" t="s">
         <v>113</v>
       </c>
+      <c r="D56" s="2"/>
       <c r="E56" t="s">
         <v>26</v>
       </c>
       <c r="F56" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="H56">
         <v>23</v>
@@ -2325,11 +2409,12 @@
       <c r="I56" t="s">
         <v>121</v>
       </c>
+      <c r="J56" s="7"/>
       <c r="K56" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="L56" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -2339,11 +2424,12 @@
       <c r="C57" t="s">
         <v>114</v>
       </c>
+      <c r="D57" s="4"/>
       <c r="E57" t="s">
         <v>26</v>
       </c>
       <c r="F57" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="H57">
         <v>22</v>
@@ -2351,11 +2437,12 @@
       <c r="I57" t="s">
         <v>122</v>
       </c>
+      <c r="J57" s="10"/>
       <c r="K57" t="s">
-        <v>156</v>
+        <v>25</v>
       </c>
       <c r="L57" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -2365,11 +2452,12 @@
       <c r="C58" t="s">
         <v>115</v>
       </c>
+      <c r="D58" s="5"/>
       <c r="E58" t="s">
         <v>26</v>
       </c>
       <c r="F58" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H58">
         <v>21</v>
@@ -2377,11 +2465,12 @@
       <c r="I58" t="s">
         <v>123</v>
       </c>
+      <c r="J58" s="18"/>
       <c r="K58" t="s">
-        <v>156</v>
+        <v>25</v>
       </c>
       <c r="L58" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -2391,11 +2480,12 @@
       <c r="C59" s="14" t="s">
         <v>5</v>
       </c>
+      <c r="D59" s="5"/>
       <c r="H59">
         <v>20</v>
       </c>
       <c r="I59" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -2405,11 +2495,12 @@
       <c r="C60" s="14" t="s">
         <v>124</v>
       </c>
+      <c r="D60" s="15"/>
       <c r="H60">
         <v>19</v>
       </c>
       <c r="I60" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -2419,9 +2510,9 @@
       <c r="C61" t="s">
         <v>49</v>
       </c>
-      <c r="D61" s="15"/>
+      <c r="D61" s="18"/>
       <c r="E61" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F61" t="s">
         <v>49</v>
@@ -2432,9 +2523,9 @@
       <c r="I61" t="s">
         <v>33</v>
       </c>
-      <c r="J61" s="7"/>
+      <c r="J61" s="12"/>
       <c r="K61" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="L61" t="s">
         <v>33</v>
@@ -2447,9 +2538,9 @@
       <c r="C62" t="s">
         <v>30</v>
       </c>
-      <c r="D62" s="2"/>
+      <c r="D62" s="10"/>
       <c r="E62" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F62" t="s">
         <v>30</v>
@@ -2458,7 +2549,7 @@
         <v>17</v>
       </c>
       <c r="I62" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -2468,9 +2559,9 @@
       <c r="C63" t="s">
         <v>125</v>
       </c>
-      <c r="D63" s="4"/>
+      <c r="D63" s="7"/>
       <c r="E63" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F63" t="s">
         <v>31</v>
@@ -2479,7 +2570,7 @@
         <v>16</v>
       </c>
       <c r="I63" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -2489,9 +2580,9 @@
       <c r="C64" t="s">
         <v>126</v>
       </c>
-      <c r="D64" s="12"/>
+      <c r="D64" s="8"/>
       <c r="E64" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F64" t="s">
         <v>48</v>
@@ -2505,266 +2596,248 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="17" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="B67" s="17" t="s">
-        <v>142</v>
+        <v>2</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I67" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="L67" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:12">
-      <c r="B68" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F68" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G68" s="17"/>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>166</v>
+      </c>
+      <c r="D68" s="20"/>
+      <c r="H68">
+        <v>8</v>
+      </c>
+      <c r="I68" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="J68" s="5"/>
     </row>
     <row r="69" spans="1:12">
       <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="D69" s="3"/>
-      <c r="E69" t="s">
-        <v>135</v>
-      </c>
-      <c r="F69" t="s">
-        <v>10</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C69" t="s">
+        <v>167</v>
+      </c>
+      <c r="D69" s="20"/>
+      <c r="H69">
+        <v>7</v>
+      </c>
+      <c r="I69" t="s">
+        <v>171</v>
+      </c>
+      <c r="J69" s="13"/>
     </row>
     <row r="70" spans="1:12">
       <c r="B70">
-        <v>2</v>
-      </c>
-      <c r="D70" s="2"/>
-      <c r="E70" t="s">
-        <v>135</v>
-      </c>
-      <c r="F70" t="s">
-        <v>30</v>
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>168</v>
+      </c>
+      <c r="D70" s="20"/>
+      <c r="H70">
+        <v>6</v>
+      </c>
+      <c r="I70" t="s">
+        <v>172</v>
+      </c>
+      <c r="J70" s="2"/>
+      <c r="K70" t="s">
+        <v>174</v>
+      </c>
+      <c r="L70" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="71" spans="1:12">
       <c r="B71">
-        <v>3</v>
-      </c>
-      <c r="D71" s="4"/>
-      <c r="E71" t="s">
-        <v>135</v>
-      </c>
-      <c r="F71" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12">
-      <c r="B72">
         <v>4</v>
       </c>
-      <c r="D72" s="8"/>
-      <c r="E72" t="s">
-        <v>135</v>
-      </c>
-      <c r="F72" t="s">
-        <v>98</v>
-      </c>
-    </row>
+      <c r="C71" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D71" s="22"/>
+      <c r="H71">
+        <v>5</v>
+      </c>
+      <c r="I71" t="s">
+        <v>173</v>
+      </c>
+      <c r="J71" s="4"/>
+      <c r="K71" t="s">
+        <v>174</v>
+      </c>
+      <c r="L71" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" s="13" customFormat="1"/>
     <row r="73" spans="1:12">
-      <c r="B73">
-        <v>5</v>
-      </c>
-      <c r="D73" s="12"/>
-      <c r="E73" t="s">
-        <v>135</v>
-      </c>
-      <c r="F73" t="s">
-        <v>97</v>
+      <c r="A73" s="17" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:12">
-      <c r="B74">
-        <v>6</v>
-      </c>
-      <c r="D74" s="7"/>
-      <c r="E74" t="s">
-        <v>135</v>
-      </c>
-      <c r="F74" t="s">
-        <v>99</v>
+      <c r="B74" s="17" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:12">
-      <c r="B75">
-        <v>7</v>
-      </c>
-      <c r="D75" s="10"/>
-      <c r="E75" t="s">
-        <v>135</v>
-      </c>
-      <c r="F75" t="s">
-        <v>100</v>
-      </c>
+      <c r="B75" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G75" s="17"/>
     </row>
     <row r="76" spans="1:12">
       <c r="B76">
-        <v>8</v>
-      </c>
-      <c r="D76" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="D76" s="3"/>
       <c r="E76" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F76" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:12">
-      <c r="B77" s="17"/>
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" t="s">
+        <v>129</v>
+      </c>
+      <c r="F77" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="78" spans="1:12">
-      <c r="B78" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="17"/>
-      <c r="J78" s="17"/>
-      <c r="K78" s="17"/>
-      <c r="L78" s="17"/>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="D78" s="4"/>
+      <c r="E78" t="s">
+        <v>129</v>
+      </c>
+      <c r="F78" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="79" spans="1:12">
-      <c r="B79" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C79" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F79" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G79" s="17"/>
-      <c r="H79" s="17"/>
-      <c r="I79" s="17"/>
-      <c r="J79" s="17"/>
-      <c r="K79" s="17"/>
-      <c r="L79" s="17"/>
+      <c r="B79">
+        <v>4</v>
+      </c>
+      <c r="D79" s="8"/>
+      <c r="E79" t="s">
+        <v>129</v>
+      </c>
+      <c r="F79" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="80" spans="1:12">
       <c r="B80">
-        <v>1</v>
-      </c>
-      <c r="D80" s="13"/>
+        <v>5</v>
+      </c>
+      <c r="D80" s="12"/>
       <c r="E80" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F80" t="s">
-        <v>10</v>
-      </c>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="17"/>
-      <c r="K80" s="17"/>
-      <c r="L80" s="17"/>
+        <v>97</v>
+      </c>
     </row>
     <row r="81" spans="2:12">
       <c r="B81">
-        <v>2</v>
-      </c>
-      <c r="D81" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="D81" s="7"/>
       <c r="E81" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F81" t="s">
-        <v>30</v>
-      </c>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
-      <c r="J81" s="17"/>
-      <c r="K81" s="17"/>
-      <c r="L81" s="17"/>
+        <v>99</v>
+      </c>
     </row>
     <row r="82" spans="2:12">
       <c r="B82">
-        <v>3</v>
-      </c>
-      <c r="D82" s="13"/>
+        <v>7</v>
+      </c>
+      <c r="D82" s="10"/>
       <c r="E82" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F82" t="s">
-        <v>31</v>
-      </c>
-      <c r="G82" s="17"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="17"/>
-      <c r="J82" s="17"/>
-      <c r="K82" s="17"/>
-      <c r="L82" s="17"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="83" spans="2:12">
       <c r="B83">
-        <v>4</v>
-      </c>
-      <c r="D83" s="13"/>
+        <v>8</v>
+      </c>
+      <c r="D83" s="8"/>
       <c r="E83" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F83" t="s">
-        <v>98</v>
-      </c>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="17"/>
-      <c r="J83" s="17"/>
-      <c r="K83" s="17"/>
-      <c r="L83" s="17"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="84" spans="2:12">
-      <c r="B84">
-        <v>5</v>
-      </c>
-      <c r="D84" s="13"/>
-      <c r="E84" t="s">
-        <v>13</v>
-      </c>
-      <c r="F84" t="s">
-        <v>13</v>
-      </c>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="17"/>
-      <c r="K84" s="17"/>
-      <c r="L84" s="17"/>
+      <c r="B84" s="17"/>
     </row>
     <row r="85" spans="2:12">
-      <c r="B85">
-        <v>6</v>
-      </c>
-      <c r="D85" s="13"/>
-      <c r="E85" t="s">
-        <v>13</v>
-      </c>
-      <c r="F85" t="s">
-        <v>13</v>
-      </c>
+      <c r="B85" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
       <c r="G85" s="17"/>
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
@@ -2773,15 +2846,18 @@
       <c r="L85" s="17"/>
     </row>
     <row r="86" spans="2:12">
-      <c r="B86">
-        <v>7</v>
-      </c>
-      <c r="D86" s="13"/>
-      <c r="E86" t="s">
-        <v>13</v>
-      </c>
-      <c r="F86" t="s">
-        <v>13</v>
+      <c r="B86" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F86" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="G86" s="17"/>
       <c r="H86" s="17"/>
@@ -2792,21 +2868,51 @@
     </row>
     <row r="87" spans="2:12">
       <c r="B87">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D87" s="13"/>
+      <c r="E87" t="s">
+        <v>135</v>
+      </c>
       <c r="F87" t="s">
-        <v>33</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G87" s="17"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="17"/>
+      <c r="J87" s="17"/>
+      <c r="K87" s="17"/>
+      <c r="L87" s="17"/>
+    </row>
+    <row r="88" spans="2:12">
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="D88" s="13"/>
+      <c r="E88" t="s">
+        <v>135</v>
+      </c>
+      <c r="F88" t="s">
+        <v>30</v>
+      </c>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="17"/>
+      <c r="J88" s="17"/>
+      <c r="K88" s="17"/>
+      <c r="L88" s="17"/>
     </row>
     <row r="89" spans="2:12">
-      <c r="B89" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="D89" s="13"/>
+      <c r="E89" t="s">
+        <v>135</v>
+      </c>
+      <c r="F89" t="s">
+        <v>31</v>
+      </c>
       <c r="G89" s="17"/>
       <c r="H89" s="17"/>
       <c r="I89" s="17"/>
@@ -2815,18 +2921,15 @@
       <c r="L89" s="17"/>
     </row>
     <row r="90" spans="2:12">
-      <c r="B90" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C90" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F90" s="17" t="s">
-        <v>38</v>
+      <c r="B90">
+        <v>4</v>
+      </c>
+      <c r="D90" s="13"/>
+      <c r="E90" t="s">
+        <v>135</v>
+      </c>
+      <c r="F90" t="s">
+        <v>98</v>
       </c>
       <c r="G90" s="17"/>
       <c r="H90" s="17"/>
@@ -2837,14 +2940,14 @@
     </row>
     <row r="91" spans="2:12">
       <c r="B91">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" t="s">
-        <v>145</v>
+        <v>13</v>
       </c>
       <c r="F91" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G91" s="17"/>
       <c r="H91" s="17"/>
@@ -2855,14 +2958,14 @@
     </row>
     <row r="92" spans="2:12">
       <c r="B92">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" t="s">
-        <v>145</v>
+        <v>13</v>
       </c>
       <c r="F92" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="G92" s="17"/>
       <c r="H92" s="17"/>
@@ -2873,14 +2976,14 @@
     </row>
     <row r="93" spans="2:12">
       <c r="B93">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" t="s">
-        <v>145</v>
+        <v>13</v>
       </c>
       <c r="F93" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G93" s="17"/>
       <c r="H93" s="17"/>
@@ -2891,48 +2994,21 @@
     </row>
     <row r="94" spans="2:12">
       <c r="B94">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D94" s="13"/>
-      <c r="E94" t="s">
-        <v>13</v>
-      </c>
-      <c r="G94" s="17"/>
-      <c r="H94" s="17"/>
-      <c r="I94" s="17"/>
-      <c r="J94" s="17"/>
-      <c r="K94" s="17"/>
-      <c r="L94" s="17"/>
-    </row>
-    <row r="95" spans="2:12">
-      <c r="B95">
-        <v>5</v>
-      </c>
-      <c r="D95" s="13"/>
-      <c r="E95" t="s">
-        <v>145</v>
-      </c>
-      <c r="F95" t="s">
-        <v>97</v>
-      </c>
-      <c r="G95" s="17"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="17"/>
-      <c r="J95" s="17"/>
-      <c r="K95" s="17"/>
-      <c r="L95" s="17"/>
+      <c r="F94" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="96" spans="2:12">
-      <c r="B96">
-        <v>6</v>
-      </c>
-      <c r="D96" s="13"/>
-      <c r="E96" t="s">
-        <v>13</v>
-      </c>
-      <c r="F96" t="s">
-        <v>13</v>
-      </c>
+      <c r="B96" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="17"/>
+      <c r="F96" s="17"/>
       <c r="G96" s="17"/>
       <c r="H96" s="17"/>
       <c r="I96" s="17"/>
@@ -2941,15 +3017,18 @@
       <c r="L96" s="17"/>
     </row>
     <row r="97" spans="2:12">
-      <c r="B97">
-        <v>7</v>
-      </c>
-      <c r="D97" s="13"/>
-      <c r="E97" t="s">
-        <v>13</v>
-      </c>
-      <c r="F97" t="s">
-        <v>13</v>
+      <c r="B97" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F97" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="G97" s="17"/>
       <c r="H97" s="17"/>
@@ -2960,20 +3039,51 @@
     </row>
     <row r="98" spans="2:12">
       <c r="B98">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="D98" s="13"/>
+      <c r="E98" t="s">
+        <v>139</v>
       </c>
       <c r="F98" t="s">
-        <v>33</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G98" s="17"/>
+      <c r="H98" s="17"/>
+      <c r="I98" s="17"/>
+      <c r="J98" s="17"/>
+      <c r="K98" s="17"/>
+      <c r="L98" s="17"/>
+    </row>
+    <row r="99" spans="2:12">
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="D99" s="13"/>
+      <c r="E99" t="s">
+        <v>139</v>
+      </c>
+      <c r="F99" t="s">
+        <v>30</v>
+      </c>
+      <c r="G99" s="17"/>
+      <c r="H99" s="17"/>
+      <c r="I99" s="17"/>
+      <c r="J99" s="17"/>
+      <c r="K99" s="17"/>
+      <c r="L99" s="17"/>
     </row>
     <row r="100" spans="2:12">
-      <c r="B100" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C100" s="17"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="17"/>
-      <c r="F100" s="17"/>
+      <c r="B100">
+        <v>3</v>
+      </c>
+      <c r="D100" s="13"/>
+      <c r="E100" t="s">
+        <v>139</v>
+      </c>
+      <c r="F100" t="s">
+        <v>31</v>
+      </c>
       <c r="G100" s="17"/>
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
@@ -2982,18 +3092,12 @@
       <c r="L100" s="17"/>
     </row>
     <row r="101" spans="2:12">
-      <c r="B101" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C101" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F101" s="17" t="s">
-        <v>38</v>
+      <c r="B101">
+        <v>4</v>
+      </c>
+      <c r="D101" s="13"/>
+      <c r="E101" t="s">
+        <v>13</v>
       </c>
       <c r="G101" s="17"/>
       <c r="H101" s="17"/>
@@ -3004,14 +3108,14 @@
     </row>
     <row r="102" spans="2:12">
       <c r="B102">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D102" s="13"/>
       <c r="E102" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F102" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="G102" s="17"/>
       <c r="H102" s="17"/>
@@ -3022,14 +3126,14 @@
     </row>
     <row r="103" spans="2:12">
       <c r="B103">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D103" s="13"/>
       <c r="E103" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="F103" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="G103" s="17"/>
       <c r="H103" s="17"/>
@@ -3040,14 +3144,14 @@
     </row>
     <row r="104" spans="2:12">
       <c r="B104">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D104" s="13"/>
       <c r="E104" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="F104" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G104" s="17"/>
       <c r="H104" s="17"/>
@@ -3058,45 +3162,20 @@
     </row>
     <row r="105" spans="2:12">
       <c r="B105">
-        <v>4</v>
-      </c>
-      <c r="D105" s="13"/>
-      <c r="E105" t="s">
-        <v>13</v>
-      </c>
-      <c r="G105" s="17"/>
-      <c r="H105" s="17"/>
-      <c r="I105" s="17"/>
-      <c r="J105" s="17"/>
-      <c r="K105" s="17"/>
-      <c r="L105" s="17"/>
-    </row>
-    <row r="106" spans="2:12">
-      <c r="B106">
-        <v>5</v>
-      </c>
-      <c r="D106" s="13"/>
-      <c r="E106" t="s">
-        <v>13</v>
-      </c>
-      <c r="G106" s="17"/>
-      <c r="H106" s="17"/>
-      <c r="I106" s="17"/>
-      <c r="J106" s="17"/>
-      <c r="K106" s="17"/>
-      <c r="L106" s="17"/>
+        <v>8</v>
+      </c>
+      <c r="F105" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="107" spans="2:12">
-      <c r="B107">
-        <v>6</v>
-      </c>
-      <c r="D107" s="13"/>
-      <c r="E107" t="s">
-        <v>147</v>
-      </c>
-      <c r="F107" t="s">
-        <v>99</v>
-      </c>
+      <c r="B107" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="17"/>
       <c r="G107" s="17"/>
       <c r="H107" s="17"/>
       <c r="I107" s="17"/>
@@ -3105,15 +3184,18 @@
       <c r="L107" s="17"/>
     </row>
     <row r="108" spans="2:12">
-      <c r="B108">
-        <v>7</v>
-      </c>
-      <c r="D108" s="13"/>
-      <c r="E108" t="s">
-        <v>147</v>
-      </c>
-      <c r="F108" t="s">
-        <v>100</v>
+      <c r="B108" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D108" s="17"/>
+      <c r="E108" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F108" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="G108" s="17"/>
       <c r="H108" s="17"/>
@@ -3124,16 +3206,136 @@
     </row>
     <row r="109" spans="2:12">
       <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="D109" s="13"/>
+      <c r="E109" t="s">
+        <v>141</v>
+      </c>
+      <c r="F109" t="s">
+        <v>10</v>
+      </c>
+      <c r="G109" s="17"/>
+      <c r="H109" s="17"/>
+      <c r="I109" s="17"/>
+      <c r="J109" s="17"/>
+      <c r="K109" s="17"/>
+      <c r="L109" s="17"/>
+    </row>
+    <row r="110" spans="2:12">
+      <c r="B110">
+        <v>2</v>
+      </c>
+      <c r="D110" s="13"/>
+      <c r="E110" t="s">
+        <v>141</v>
+      </c>
+      <c r="F110" t="s">
+        <v>30</v>
+      </c>
+      <c r="G110" s="17"/>
+      <c r="H110" s="17"/>
+      <c r="I110" s="17"/>
+      <c r="J110" s="17"/>
+      <c r="K110" s="17"/>
+      <c r="L110" s="17"/>
+    </row>
+    <row r="111" spans="2:12">
+      <c r="B111">
+        <v>3</v>
+      </c>
+      <c r="D111" s="13"/>
+      <c r="E111" t="s">
+        <v>141</v>
+      </c>
+      <c r="F111" t="s">
+        <v>31</v>
+      </c>
+      <c r="G111" s="17"/>
+      <c r="H111" s="17"/>
+      <c r="I111" s="17"/>
+      <c r="J111" s="17"/>
+      <c r="K111" s="17"/>
+      <c r="L111" s="17"/>
+    </row>
+    <row r="112" spans="2:12">
+      <c r="B112">
+        <v>4</v>
+      </c>
+      <c r="D112" s="13"/>
+      <c r="E112" t="s">
+        <v>13</v>
+      </c>
+      <c r="G112" s="17"/>
+      <c r="H112" s="17"/>
+      <c r="I112" s="17"/>
+      <c r="J112" s="17"/>
+      <c r="K112" s="17"/>
+      <c r="L112" s="17"/>
+    </row>
+    <row r="113" spans="2:12">
+      <c r="B113">
+        <v>5</v>
+      </c>
+      <c r="D113" s="13"/>
+      <c r="E113" t="s">
+        <v>13</v>
+      </c>
+      <c r="G113" s="17"/>
+      <c r="H113" s="17"/>
+      <c r="I113" s="17"/>
+      <c r="J113" s="17"/>
+      <c r="K113" s="17"/>
+      <c r="L113" s="17"/>
+    </row>
+    <row r="114" spans="2:12">
+      <c r="B114">
+        <v>6</v>
+      </c>
+      <c r="D114" s="13"/>
+      <c r="E114" t="s">
+        <v>141</v>
+      </c>
+      <c r="F114" t="s">
+        <v>99</v>
+      </c>
+      <c r="G114" s="17"/>
+      <c r="H114" s="17"/>
+      <c r="I114" s="17"/>
+      <c r="J114" s="17"/>
+      <c r="K114" s="17"/>
+      <c r="L114" s="17"/>
+    </row>
+    <row r="115" spans="2:12">
+      <c r="B115">
+        <v>7</v>
+      </c>
+      <c r="D115" s="13"/>
+      <c r="E115" t="s">
+        <v>141</v>
+      </c>
+      <c r="F115" t="s">
+        <v>100</v>
+      </c>
+      <c r="G115" s="17"/>
+      <c r="H115" s="17"/>
+      <c r="I115" s="17"/>
+      <c r="J115" s="17"/>
+      <c r="K115" s="17"/>
+      <c r="L115" s="17"/>
+    </row>
+    <row r="116" spans="2:12">
+      <c r="B116">
         <v>8</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F116" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="2:12">
-      <c r="B111" s="13"/>
-      <c r="C111" s="14"/>
-      <c r="D111" t="s">
+    <row r="118" spans="2:12">
+      <c r="B118" s="13"/>
+      <c r="C118" s="14"/>
+      <c r="D118" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>